<commit_message>
run all the GLB datasets
</commit_message>
<xml_diff>
--- a/强力单因子列表.xlsx
+++ b/强力单因子列表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelxu/My_Document/Michael/金融/量化/WorldQuant/alpha_creation_engine-main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A7453A8-9F70-4A45-A879-1753CE3B739B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9878FE4-8FB4-754F-A9B8-1688515449F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9860" yWindow="500" windowWidth="20860" windowHeight="17720" xr2:uid="{29EBAAB1-C742-0741-A0AC-8BD67BDD565A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="55">
   <si>
     <t>Expression</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -191,6 +191,41 @@
   </si>
   <si>
     <t>ts_zscore(star_eps_surprise_prediction_fy2,40)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ts_zscore(anl69_ebit_best_eeps_cur_yr,14)</t>
+  </si>
+  <si>
+    <t>ts_zscore(anl69_sales_best_eeps_nxt_yr,20)</t>
+  </si>
+  <si>
+    <t>ts_zscore(anl69_roa_best_eeps_cur_yr,20)</t>
+  </si>
+  <si>
+    <t>analyst69</t>
+  </si>
+  <si>
+    <t>-ts_zscore(fnd17_spfcfrpmtt,260)</t>
+  </si>
+  <si>
+    <t>ts_zscore(fnd17_dai,170)</t>
+  </si>
+  <si>
+    <t>ts_zscore(fnd17_ebitda2ev_ttm,160)</t>
+  </si>
+  <si>
+    <t>ts_zscore(fnd17_rhsfcfmtt,80)</t>
+  </si>
+  <si>
+    <t>Passes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ts_zscore(rsk70_mfm2_gemtrd_anlystsn,50)</t>
+  </si>
+  <si>
+    <t>ts_rank(fnd23_intfvmfm2_tibs,40)+ts_rank(fnd23_intfvmfm2_tibs,55)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -215,7 +250,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -240,6 +275,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -255,7 +302,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -267,6 +314,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -602,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B93DFF34-AD34-234D-887E-B203DAABE910}">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -614,9 +670,10 @@
     <col min="2" max="2" width="59.83203125" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" customWidth="1"/>
     <col min="4" max="4" width="20.5" customWidth="1"/>
+    <col min="5" max="5" width="20.5" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -629,11 +686,14 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -646,11 +706,11 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -664,7 +724,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="B4" s="1" t="s">
         <v>28</v>
       </c>
@@ -675,7 +735,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="B5" s="1" t="s">
         <v>29</v>
       </c>
@@ -686,7 +746,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="B6" s="1" t="s">
         <v>30</v>
       </c>
@@ -697,7 +757,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="B7" s="1" t="s">
         <v>31</v>
       </c>
@@ -708,7 +768,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="B8" s="1" t="s">
         <v>32</v>
       </c>
@@ -719,7 +779,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="B9" s="2" t="s">
         <v>33</v>
       </c>
@@ -730,7 +790,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="B10" s="2" t="s">
         <v>34</v>
       </c>
@@ -741,22 +801,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="C11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:6">
       <c r="C12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6">
       <c r="C13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -769,8 +829,11 @@
       <c r="D14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -784,7 +847,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -798,7 +861,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -812,7 +875,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -826,7 +889,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -840,18 +903,66 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
       </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
       <c r="D20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="F20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -864,8 +975,11 @@
       <c r="D26" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="F26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="B27" t="s">
         <v>22</v>
       </c>
@@ -876,102 +990,162 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
-      <c r="B28" t="s">
+    <row r="28" spans="1:6">
+      <c r="B28" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="B29" t="s">
         <v>23</v>
       </c>
-      <c r="C28" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" t="s">
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="B30" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="B31" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="B32" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
         <v>24</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>25</v>
       </c>
-      <c r="C33" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="B34" t="s">
+      <c r="C34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="B35" t="s">
         <v>26</v>
       </c>
-      <c r="C34" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="B35" t="s">
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="B36" t="s">
         <v>27</v>
       </c>
-      <c r="C35" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" t="s">
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B40" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C39" t="s">
-        <v>4</v>
-      </c>
-      <c r="D39" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="B40" s="1" t="s">
+      <c r="C40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="B41" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C40" t="s">
-        <v>4</v>
-      </c>
-      <c r="D40" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="B41" s="2" t="s">
+      <c r="C41" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="B42" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C41" t="s">
-        <v>4</v>
-      </c>
-      <c r="D41" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="B42" t="s">
+      <c r="C42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="B43" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
-      <c r="B43" t="s">
+    <row r="44" spans="1:6">
+      <c r="B44" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
-      <c r="B44" t="s">
+    <row r="45" spans="1:6">
+      <c r="B45" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="B47" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F47" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5">
+      <c r="B53" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E53" s="6">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>